<commit_message>
FW update and Board correction
P4 should be a SM shrouded male header, not through  hole
</commit_message>
<xml_diff>
--- a/RGB-IR Backlight 7x7/Electrical/7x7RGB-IR-J010129B.xlsx
+++ b/RGB-IR Backlight 7x7/Electrical/7x7RGB-IR-J010129B.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\ID&amp;F\RGB LEDs\7_INCH\SEPARATE_LEDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69648834-ECD0-4108-A11E-55214A4B028D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C6907F-C077-4668-A485-C89C5BD974E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="1095" windowWidth="30960" windowHeight="14250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="600" windowWidth="29490" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="J005794_RGB_IR" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">J005794_RGB_IR!$A$1:$M$21</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">J005794_RGB_IR!$A$1:$M$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="136">
   <si>
     <t>Qty</t>
   </si>
@@ -117,9 +117,6 @@
     <t>Infrared (IR) Emitter 860nm 1.5V 100mA 9mW/sr @ 100mA 140° 2-SMD, Flat Lead</t>
   </si>
   <si>
-    <t>Hirose</t>
-  </si>
-  <si>
     <t>UUR1J470MNL1GS</t>
   </si>
   <si>
@@ -183,12 +180,6 @@
     <t>DK</t>
   </si>
   <si>
-    <t>J2</t>
-  </si>
-  <si>
-    <t>CONN HEADER 3POS 1.25MM SMD GOLD</t>
-  </si>
-  <si>
     <t>RES SMD 10 OHM 1% 1/4W 1206</t>
   </si>
   <si>
@@ -372,12 +363,6 @@
     <t>AE11242-ND</t>
   </si>
   <si>
-    <t>DF13C-3P-1.25V(76)</t>
-  </si>
-  <si>
-    <t>H126463-ND</t>
-  </si>
-  <si>
     <t>Triangle on part goes to small circle on board by pin 1</t>
   </si>
   <si>
@@ -439,6 +424,24 @@
   </si>
   <si>
     <t>NOTE: Place LEDS at each location using silkscreen markings 'R', 'G', 'B'.</t>
+  </si>
+  <si>
+    <t>2x3 header</t>
+  </si>
+  <si>
+    <t>Connector Header Surface Mount 6 position 0.100" (2.54mm)</t>
+  </si>
+  <si>
+    <t>HTSS-103-01-T-DV</t>
+  </si>
+  <si>
+    <t>Samtec Inc.</t>
+  </si>
+  <si>
+    <t>HTSS-103-01-T-DV-ND</t>
+  </si>
+  <si>
+    <t>P4</t>
   </si>
 </sst>
 </file>
@@ -1319,10 +1322,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1346,7 +1349,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -1396,13 +1399,13 @@
         <v>10</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -1410,28 +1413,28 @@
         <v>3</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="I3" s="2">
         <v>0.52</v>
       </c>
       <c r="J3" s="2">
-        <f t="shared" ref="J3:J24" si="0">A3*I3</f>
+        <f t="shared" ref="J3:J25" si="0">A3*I3</f>
         <v>1.56</v>
       </c>
       <c r="L3" s="4">
@@ -1447,160 +1450,163 @@
         <v>4.68</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="330" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>1</v>
+        <v>259</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>112</v>
+        <v>23</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0.73</v>
+        <v>25</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" si="0"/>
-        <v>0.73</v>
+        <v>0</v>
       </c>
       <c r="L4" s="4">
-        <f t="shared" ref="L4:L24" si="1">A4*10</f>
-        <v>10</v>
+        <f t="shared" ref="L4:L25" si="1">A4*10</f>
+        <v>2590</v>
       </c>
       <c r="M4" s="2">
-        <f t="shared" ref="M4:M24" si="2">J4*10</f>
-        <v>7.3</v>
+        <f t="shared" ref="M4:M25" si="2">J4*10</f>
+        <v>0</v>
       </c>
       <c r="N4" s="2">
-        <f t="shared" ref="N4:N24" si="3">J4*3</f>
-        <v>2.19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="330" x14ac:dyDescent="0.25">
+        <f t="shared" ref="N4:N23" si="3">J4*3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>259</v>
+        <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>25</v>
+        <v>33</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1.89</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.89</v>
       </c>
       <c r="L5" s="4">
         <f t="shared" si="1"/>
-        <v>2590</v>
+        <v>10</v>
       </c>
       <c r="M5" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="N5" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.67</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="I6" s="2">
-        <v>1.89</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" si="0"/>
-        <v>1.89</v>
+        <v>0.112</v>
       </c>
       <c r="L6" s="4">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="M6" s="2">
         <f t="shared" si="2"/>
-        <v>18.899999999999999</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="N6" s="2">
         <f t="shared" si="3"/>
-        <v>5.67</v>
+        <v>0.33600000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="B7" s="3">
-        <v>0.1</v>
+      <c r="B7" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="I7" s="2">
-        <v>2.8000000000000001E-2</v>
+        <v>0.13</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" si="0"/>
-        <v>0.112</v>
+        <v>0.52</v>
       </c>
       <c r="L7" s="4">
         <f t="shared" si="1"/>
@@ -1608,673 +1614,667 @@
       </c>
       <c r="M7" s="2">
         <f t="shared" si="2"/>
-        <v>1.1200000000000001</v>
+        <v>5.2</v>
       </c>
       <c r="N7" s="2">
         <f t="shared" si="3"/>
-        <v>0.33600000000000002</v>
+        <v>1.56</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="H8" s="5" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="I8" s="2">
-        <v>0.13</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" si="0"/>
-        <v>0.52</v>
+        <v>4.5599999999999996</v>
       </c>
       <c r="L8" s="4">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="M8" s="2">
         <f t="shared" si="2"/>
-        <v>5.2</v>
+        <v>45.599999999999994</v>
       </c>
       <c r="N8" s="2">
         <f t="shared" si="3"/>
-        <v>1.56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>13.68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>61</v>
+        <v>111</v>
       </c>
       <c r="I9" s="2">
-        <v>0.56999999999999995</v>
+        <v>0.24</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" si="0"/>
-        <v>4.5599999999999996</v>
+        <v>0.96</v>
       </c>
       <c r="L9" s="4">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="M9" s="2">
         <f t="shared" si="2"/>
-        <v>45.599999999999994</v>
+        <v>9.6</v>
       </c>
       <c r="N9" s="2">
         <f t="shared" si="3"/>
-        <v>13.68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2.88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="F10" s="5" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="I10" s="2">
-        <v>0.24</v>
+        <v>0.34</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" si="0"/>
-        <v>0.96</v>
+        <v>8.16</v>
       </c>
       <c r="L10" s="4">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>240</v>
       </c>
       <c r="M10" s="2">
         <f t="shared" si="2"/>
-        <v>9.6</v>
+        <v>81.599999999999994</v>
       </c>
       <c r="N10" s="2">
         <f t="shared" si="3"/>
-        <v>2.88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24.48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="I11" s="2">
-        <v>0.34</v>
+        <v>0.66400000000000003</v>
       </c>
       <c r="J11" s="2">
         <f t="shared" si="0"/>
-        <v>8.16</v>
+        <v>2.6560000000000001</v>
       </c>
       <c r="L11" s="4">
         <f t="shared" si="1"/>
-        <v>240</v>
+        <v>40</v>
       </c>
       <c r="M11" s="2">
         <f t="shared" si="2"/>
-        <v>81.599999999999994</v>
+        <v>26.560000000000002</v>
       </c>
       <c r="N11" s="2">
         <f t="shared" si="3"/>
-        <v>24.48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <v>7.968</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="I12" s="2">
-        <v>0.66400000000000003</v>
+        <v>0.123</v>
       </c>
       <c r="J12" s="2">
         <f t="shared" si="0"/>
-        <v>2.6560000000000001</v>
+        <v>1.968</v>
       </c>
       <c r="L12" s="4">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>160</v>
       </c>
       <c r="M12" s="2">
         <f t="shared" si="2"/>
-        <v>26.560000000000002</v>
+        <v>19.68</v>
       </c>
       <c r="N12" s="2">
         <f t="shared" si="3"/>
-        <v>7.968</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5.9039999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>87</v>
+        <v>19</v>
       </c>
       <c r="E13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="H13" s="5" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="I13" s="2">
-        <v>0.123</v>
+        <v>0.1</v>
       </c>
       <c r="J13" s="2">
         <f t="shared" si="0"/>
-        <v>1.968</v>
+        <v>0.4</v>
       </c>
       <c r="L13" s="4">
         <f t="shared" si="1"/>
-        <v>160</v>
+        <v>40</v>
       </c>
       <c r="M13" s="2">
         <f t="shared" si="2"/>
-        <v>19.68</v>
+        <v>4</v>
       </c>
       <c r="N13" s="2">
         <f t="shared" si="3"/>
-        <v>5.9039999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+        <v>1.2000000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>4</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="B14" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14"/>
       <c r="D14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="I14" s="2">
-        <v>0.1</v>
+        <v>85</v>
+      </c>
+      <c r="E14" t="s">
+        <v>88</v>
+      </c>
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14">
+        <v>2.38</v>
       </c>
       <c r="J14" s="2">
+        <f t="shared" ref="J14" si="4">A14*I14</f>
+        <v>9.52</v>
+      </c>
+      <c r="K14" t="s">
+        <v>89</v>
+      </c>
+      <c r="L14" t="s">
+        <v>89</v>
+      </c>
+      <c r="M14" t="s">
+        <v>89</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="3"/>
+        <v>28.56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>4</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="J15" s="2">
         <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="L14" s="4">
+        <v>1</v>
+      </c>
+      <c r="L15" s="4">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M15" s="2">
         <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="N14" s="2">
-        <f t="shared" si="3"/>
-        <v>1.2000000000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>4</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C15"/>
-      <c r="D15" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E15" t="s">
-        <v>91</v>
-      </c>
-      <c r="F15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" t="s">
-        <v>48</v>
-      </c>
-      <c r="H15" t="s">
-        <v>36</v>
-      </c>
-      <c r="I15">
-        <v>2.38</v>
-      </c>
-      <c r="J15" s="2">
-        <f t="shared" ref="J15" si="4">A15*I15</f>
-        <v>9.52</v>
-      </c>
-      <c r="K15" t="s">
-        <v>92</v>
-      </c>
-      <c r="L15" t="s">
-        <v>92</v>
-      </c>
-      <c r="M15" t="s">
-        <v>92</v>
+        <v>10</v>
       </c>
       <c r="N15" s="2">
         <f t="shared" si="3"/>
-        <v>28.56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>38</v>
+        <v>65</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="H16" t="s">
-        <v>39</v>
+        <v>47</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="I16" s="2">
-        <v>0.25</v>
+        <v>0.89</v>
       </c>
       <c r="J16" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>10.68</v>
       </c>
       <c r="L16" s="4">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="M16" s="2">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>106.8</v>
       </c>
       <c r="N16" s="2">
         <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+        <v>32.04</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>40</v>
+        <v>112</v>
+      </c>
+      <c r="F17" s="5">
+        <v>5100</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>41</v>
+        <v>113</v>
       </c>
       <c r="I17" s="2">
-        <v>0.89</v>
+        <v>0.24</v>
       </c>
       <c r="J17" s="2">
         <f t="shared" si="0"/>
-        <v>10.68</v>
+        <v>3.36</v>
       </c>
       <c r="L17" s="4">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="M17" s="2">
         <f t="shared" si="2"/>
-        <v>106.8</v>
+        <v>33.6</v>
       </c>
       <c r="N17" s="2">
         <f t="shared" si="3"/>
-        <v>32.04</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>10.08</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>94</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="F18" s="5">
-        <v>5100</v>
+        <v>80</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="I18" s="2">
-        <v>0.24</v>
+        <v>0.1</v>
       </c>
       <c r="J18" s="2">
         <f t="shared" si="0"/>
-        <v>3.36</v>
+        <v>1.8</v>
       </c>
       <c r="L18" s="4">
         <f t="shared" si="1"/>
-        <v>140</v>
+        <v>180</v>
       </c>
       <c r="M18" s="2">
         <f t="shared" si="2"/>
-        <v>33.6</v>
+        <v>18</v>
       </c>
       <c r="N18" s="2">
         <f t="shared" si="3"/>
-        <v>10.08</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I19" s="2">
-        <v>0.1</v>
+        <v>0.21</v>
       </c>
       <c r="J19" s="2">
         <f t="shared" si="0"/>
-        <v>1.8</v>
+        <v>0.21</v>
       </c>
       <c r="L19" s="4">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="M19" s="2">
+        <v>10</v>
+      </c>
+      <c r="M19" s="5">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>2.1</v>
       </c>
       <c r="N19" s="2">
         <f t="shared" si="3"/>
-        <v>5.4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="I20" s="2">
-        <v>0.21</v>
+        <v>1.5</v>
       </c>
       <c r="J20" s="2">
         <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>3</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="L20" s="4">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="M20" s="5">
         <f t="shared" si="2"/>
-        <v>2.1</v>
+        <v>30</v>
       </c>
       <c r="N20" s="2">
         <f t="shared" si="3"/>
-        <v>0.63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>48</v>
+        <v>124</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="I21" s="2">
-        <v>1.5</v>
+        <v>1.57</v>
       </c>
       <c r="J21" s="2">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="K21" s="5" t="s">
-        <v>114</v>
+        <v>100.48</v>
       </c>
       <c r="L21" s="4">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>640</v>
       </c>
       <c r="M21" s="5">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>1004.8000000000001</v>
       </c>
       <c r="N21" s="2">
         <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+        <v>301.44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>64</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>129</v>
-      </c>
       <c r="H22" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I22" s="2">
-        <v>1.57</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="J22" s="2">
         <f t="shared" si="0"/>
-        <v>100.48</v>
+        <v>72.959999999999994</v>
       </c>
       <c r="L22" s="4">
         <f t="shared" si="1"/>
@@ -2282,31 +2282,28 @@
       </c>
       <c r="M22" s="5">
         <f t="shared" si="2"/>
-        <v>1004.8000000000001</v>
+        <v>729.59999999999991</v>
       </c>
       <c r="N22" s="2">
         <f t="shared" si="3"/>
-        <v>301.44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>218.88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>64</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>121</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="I23" s="2">
         <v>1.1399999999999999</v>
@@ -2319,7 +2316,7 @@
         <f t="shared" si="1"/>
         <v>640</v>
       </c>
-      <c r="M23" s="5">
+      <c r="M23" s="2">
         <f t="shared" si="2"/>
         <v>729.59999999999991</v>
       </c>
@@ -2328,51 +2325,72 @@
         <v>218.88</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
-        <v>64</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D24" s="5" t="s">
+    <row r="24" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C24" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="N24" s="5">
+        <v>350</v>
+      </c>
+      <c r="O24" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>1</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="F24" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="I24" s="2">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="J24" s="2">
+      <c r="F25" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="I25" s="2">
+        <v>3.06</v>
+      </c>
+      <c r="J25" s="2">
         <f t="shared" si="0"/>
-        <v>72.959999999999994</v>
-      </c>
-      <c r="L24" s="4">
+        <v>3.06</v>
+      </c>
+      <c r="L25" s="4">
         <f t="shared" si="1"/>
-        <v>640</v>
-      </c>
-      <c r="M24" s="2">
+        <v>10</v>
+      </c>
+      <c r="M25" s="2">
         <f t="shared" si="2"/>
-        <v>729.59999999999991</v>
-      </c>
-      <c r="N24" s="2">
-        <f t="shared" si="3"/>
-        <v>218.88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C25" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="N25" s="5">
-        <v>350</v>
-      </c>
-      <c r="O25" s="5" t="s">
-        <v>128</v>
+        <v>30.6</v>
+      </c>
+      <c r="N25" s="2">
+        <f>J25*3</f>
+        <v>9.18</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -2380,34 +2398,31 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C27" s="3"/>
+      <c r="J27" s="2">
+        <f>SUM(J3:J23)</f>
+        <v>298.75599999999997</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="N27" s="2">
+        <f>SUM(N3:N25)</f>
+        <v>1255.4480000000001</v>
+      </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C28" s="3"/>
-      <c r="J28" s="2">
-        <f>SUM(J3:J24)</f>
-        <v>299.48599999999999</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L28" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="M28" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="N28" s="2">
-        <f>SUM(N3:N25)</f>
-        <v>1248.4580000000001</v>
+      <c r="N28" s="5" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N29" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C30" s="3"/>
+      <c r="C29" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>